<commit_message>
gantt update, projektdoku realisieren teil update, input validieren
</commit_message>
<xml_diff>
--- a/docs/M223_Gantt_Planung_Felix.xlsx
+++ b/docs/M223_Gantt_Planung_Felix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lara\Documents\GitHub\M223\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D3A21C-CFDD-4A95-A13F-ECB36022F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E521F6-B636-4FE3-AC18-DF05F4DC2CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="507" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1036,96 +1036,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1139,8 +1049,97 @@
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1436,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="74" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="74" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1471,35 +1470,35 @@
       <c r="A1" s="60"/>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
-      <c r="D1" s="185" t="s">
+      <c r="D1" s="190" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="178" t="s">
+      <c r="E1" s="187"/>
+      <c r="F1" s="186"/>
+      <c r="G1" s="185" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="182"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="178" t="s">
+      <c r="H1" s="187"/>
+      <c r="I1" s="186"/>
+      <c r="J1" s="185" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="182"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="178" t="s">
+      <c r="K1" s="187"/>
+      <c r="L1" s="186"/>
+      <c r="M1" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="182"/>
-      <c r="O1" s="179"/>
-      <c r="P1" s="178" t="s">
+      <c r="N1" s="187"/>
+      <c r="O1" s="186"/>
+      <c r="P1" s="185" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="182"/>
-      <c r="R1" s="179"/>
-      <c r="S1" s="178" t="s">
+      <c r="Q1" s="187"/>
+      <c r="R1" s="186"/>
+      <c r="S1" s="185" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="179"/>
+      <c r="T1" s="186"/>
       <c r="U1" s="48"/>
       <c r="V1" s="28"/>
       <c r="W1" s="28" t="s">
@@ -1507,9 +1506,9 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="67" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="167"/>
-      <c r="B2" s="168"/>
-      <c r="C2" s="169"/>
+      <c r="A2" s="196"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="198"/>
       <c r="D2" s="63" t="s">
         <v>4</v>
       </c>
@@ -1566,10 +1565,10 @@
       <c r="W2" s="28"/>
     </row>
     <row r="3" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="193" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="173" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -1593,14 +1592,14 @@
       <c r="S3" s="78"/>
       <c r="T3" s="77"/>
       <c r="U3" s="99"/>
-      <c r="V3" s="177" t="s">
+      <c r="V3" s="184" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="177"/>
+      <c r="W3" s="184"/>
     </row>
     <row r="4" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="162"/>
-      <c r="B4" s="181"/>
+      <c r="A4" s="180"/>
+      <c r="B4" s="177"/>
       <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1628,10 +1627,10 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="179" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="176" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1661,8 +1660,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="173"/>
-      <c r="B6" s="166"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="174"/>
       <c r="C6" s="19" t="s">
         <v>1</v>
       </c>
@@ -1690,8 +1689,8 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="173"/>
-      <c r="B7" s="166" t="s">
+      <c r="A7" s="179"/>
+      <c r="B7" s="174" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -1721,17 +1720,17 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="173"/>
-      <c r="B8" s="166"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="174"/>
       <c r="C8" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="192"/>
-      <c r="G8" s="190"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="160"/>
       <c r="H8" s="104"/>
-      <c r="I8" s="191"/>
+      <c r="I8" s="161"/>
       <c r="J8" s="49"/>
       <c r="K8" s="7"/>
       <c r="L8" s="36"/>
@@ -1748,8 +1747,8 @@
       <c r="W8" s="85"/>
     </row>
     <row r="9" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="173"/>
-      <c r="B9" s="180" t="s">
+      <c r="A9" s="179"/>
+      <c r="B9" s="175" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -1777,8 +1776,8 @@
       <c r="W9" s="85"/>
     </row>
     <row r="10" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="173"/>
-      <c r="B10" s="170"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="176"/>
       <c r="C10" s="19" t="s">
         <v>1</v>
       </c>
@@ -1806,8 +1805,8 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="173"/>
-      <c r="B11" s="171" t="s">
+      <c r="A11" s="179"/>
+      <c r="B11" s="178" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -1837,8 +1836,8 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="173"/>
-      <c r="B12" s="172"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="199"/>
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
@@ -1846,8 +1845,8 @@
       <c r="E12" s="118"/>
       <c r="F12" s="119"/>
       <c r="G12" s="120"/>
-      <c r="H12" s="193"/>
-      <c r="I12" s="194"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="164"/>
       <c r="J12" s="122"/>
       <c r="K12" s="123"/>
       <c r="L12" s="121"/>
@@ -1864,10 +1863,10 @@
       <c r="W12" s="113"/>
     </row>
     <row r="13" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="193" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="194" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -1895,8 +1894,8 @@
       <c r="W13" s="90"/>
     </row>
     <row r="14" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="162"/>
-      <c r="B14" s="164"/>
+      <c r="A14" s="180"/>
+      <c r="B14" s="195"/>
       <c r="C14" s="20" t="s">
         <v>1</v>
       </c>
@@ -1904,7 +1903,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="38"/>
       <c r="G14" s="37"/>
-      <c r="H14" s="195"/>
+      <c r="H14" s="165"/>
       <c r="I14" s="105"/>
       <c r="J14" s="56"/>
       <c r="K14" s="11"/>
@@ -1922,10 +1921,10 @@
       <c r="W14" s="113"/>
     </row>
     <row r="15" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="174" t="s">
+      <c r="B15" s="200" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -1953,8 +1952,8 @@
       <c r="W15" s="90"/>
     </row>
     <row r="16" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="160"/>
-      <c r="B16" s="175"/>
+      <c r="A16" s="192"/>
+      <c r="B16" s="201"/>
       <c r="C16" s="20" t="s">
         <v>1</v>
       </c>
@@ -1980,10 +1979,10 @@
       <c r="W16" s="113"/>
     </row>
     <row r="17" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="186" t="s">
+      <c r="A17" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="173" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="21" t="s">
@@ -2010,8 +2009,8 @@
       <c r="V17" s="90"/>
     </row>
     <row r="18" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="187"/>
-      <c r="B18" s="166"/>
+      <c r="A18" s="182"/>
+      <c r="B18" s="174"/>
       <c r="C18" s="19" t="s">
         <v>1</v>
       </c>
@@ -2019,9 +2018,9 @@
       <c r="E18" s="10"/>
       <c r="F18" s="36"/>
       <c r="G18" s="33"/>
-      <c r="H18" s="197"/>
-      <c r="I18" s="192"/>
-      <c r="J18" s="196"/>
+      <c r="H18" s="167"/>
+      <c r="I18" s="162"/>
+      <c r="J18" s="166"/>
       <c r="K18" s="7"/>
       <c r="L18" s="36"/>
       <c r="M18" s="49"/>
@@ -2036,8 +2035,8 @@
       <c r="V18" s="90"/>
     </row>
     <row r="19" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="187"/>
-      <c r="B19" s="170" t="s">
+      <c r="A19" s="182"/>
+      <c r="B19" s="176" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -2065,8 +2064,8 @@
       <c r="W19" s="90"/>
     </row>
     <row r="20" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="187"/>
-      <c r="B20" s="166"/>
+      <c r="A20" s="182"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="19" t="s">
         <v>1</v>
       </c>
@@ -2074,11 +2073,11 @@
       <c r="E20" s="10"/>
       <c r="G20" s="33"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="198"/>
-      <c r="K20" s="197"/>
-      <c r="L20" s="189"/>
-      <c r="M20" s="190"/>
+      <c r="I20" s="162"/>
+      <c r="J20" s="168"/>
+      <c r="K20" s="167"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="160"/>
       <c r="N20" s="104"/>
       <c r="O20" s="34"/>
       <c r="P20" s="33"/>
@@ -2088,8 +2087,8 @@
       <c r="T20" s="34"/>
     </row>
     <row r="21" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="187"/>
-      <c r="B21" s="171" t="s">
+      <c r="A21" s="182"/>
+      <c r="B21" s="178" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -2114,8 +2113,8 @@
       <c r="T21" s="50"/>
     </row>
     <row r="22" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="187"/>
-      <c r="B22" s="171"/>
+      <c r="A22" s="182"/>
+      <c r="B22" s="178"/>
       <c r="C22" s="19" t="s">
         <v>1</v>
       </c>
@@ -2125,13 +2124,13 @@
       <c r="G22" s="49"/>
       <c r="H22" s="7"/>
       <c r="I22" s="36"/>
-      <c r="J22" s="198"/>
-      <c r="K22" s="197"/>
-      <c r="L22" s="192"/>
-      <c r="M22" s="196"/>
-      <c r="N22" s="199"/>
-      <c r="O22" s="191"/>
-      <c r="P22" s="196"/>
+      <c r="J22" s="168"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="162"/>
+      <c r="M22" s="166"/>
+      <c r="N22" s="169"/>
+      <c r="O22" s="161"/>
+      <c r="P22" s="166"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="50"/>
       <c r="S22" s="35"/>
@@ -2141,8 +2140,8 @@
       <c r="W22" s="90"/>
     </row>
     <row r="23" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="187"/>
-      <c r="B23" s="166" t="s">
+      <c r="A23" s="182"/>
+      <c r="B23" s="174" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -2170,8 +2169,8 @@
       <c r="W23" s="90"/>
     </row>
     <row r="24" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="187"/>
-      <c r="B24" s="166"/>
+      <c r="A24" s="182"/>
+      <c r="B24" s="174"/>
       <c r="C24" s="19" t="s">
         <v>1</v>
       </c>
@@ -2184,9 +2183,9 @@
       <c r="J24" s="49"/>
       <c r="K24" s="7"/>
       <c r="L24" s="36"/>
-      <c r="M24" s="190"/>
+      <c r="M24" s="160"/>
       <c r="N24" s="104"/>
-      <c r="O24" s="189"/>
+      <c r="O24" s="159"/>
       <c r="P24" s="35"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="50"/>
@@ -2197,8 +2196,8 @@
       <c r="W24" s="90"/>
     </row>
     <row r="25" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="187"/>
-      <c r="B25" s="166" t="s">
+      <c r="A25" s="182"/>
+      <c r="B25" s="174" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -2226,8 +2225,8 @@
       <c r="W25" s="90"/>
     </row>
     <row r="26" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="187"/>
-      <c r="B26" s="166"/>
+      <c r="A26" s="182"/>
+      <c r="B26" s="174"/>
       <c r="C26" s="19" t="s">
         <v>1</v>
       </c>
@@ -2235,8 +2234,8 @@
       <c r="E26" s="10"/>
       <c r="M26" s="33"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="189"/>
-      <c r="P26" s="190"/>
+      <c r="O26" s="159"/>
+      <c r="P26" s="160"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="34"/>
       <c r="S26" s="33"/>
@@ -2245,8 +2244,8 @@
       <c r="V26" s="90"/>
     </row>
     <row r="27" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="187"/>
-      <c r="B27" s="166" t="s">
+      <c r="A27" s="182"/>
+      <c r="B27" s="174" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="19" t="s">
@@ -2273,8 +2272,8 @@
       <c r="V27" s="90"/>
     </row>
     <row r="28" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="188"/>
-      <c r="B28" s="181"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="177"/>
       <c r="C28" s="20" t="s">
         <v>1</v>
       </c>
@@ -2290,19 +2289,19 @@
       <c r="M28" s="54"/>
       <c r="N28" s="30"/>
       <c r="O28" s="45"/>
-      <c r="P28" s="200"/>
+      <c r="P28" s="170"/>
       <c r="Q28" s="202"/>
-      <c r="R28" s="203"/>
+      <c r="R28" s="171"/>
       <c r="S28" s="37"/>
       <c r="T28" s="76"/>
       <c r="U28" s="100"/>
       <c r="V28" s="90"/>
     </row>
     <row r="29" spans="1:23" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="187" t="s">
+      <c r="A29" s="182" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="165" t="s">
+      <c r="B29" s="173" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -2328,8 +2327,8 @@
       <c r="V29" s="90"/>
     </row>
     <row r="30" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="187"/>
-      <c r="B30" s="166"/>
+      <c r="A30" s="182"/>
+      <c r="B30" s="174"/>
       <c r="C30" s="19" t="s">
         <v>1</v>
       </c>
@@ -2342,8 +2341,8 @@
       <c r="J30" s="35"/>
       <c r="K30" s="9"/>
       <c r="L30" s="50"/>
-      <c r="M30" s="196"/>
-      <c r="N30" s="199"/>
+      <c r="M30" s="166"/>
+      <c r="N30" s="169"/>
       <c r="O30" s="50"/>
       <c r="P30" s="35"/>
       <c r="Q30" s="9"/>
@@ -2354,8 +2353,8 @@
       <c r="V30" s="90"/>
     </row>
     <row r="31" spans="1:23" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="187"/>
-      <c r="B31" s="170" t="s">
+      <c r="A31" s="182"/>
+      <c r="B31" s="176" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="18" t="s">
@@ -2381,8 +2380,8 @@
       <c r="V31" s="90"/>
     </row>
     <row r="32" spans="1:23" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="188"/>
-      <c r="B32" s="181"/>
+      <c r="A32" s="183"/>
+      <c r="B32" s="177"/>
       <c r="C32" s="20" t="s">
         <v>1</v>
       </c>
@@ -2397,7 +2396,7 @@
       <c r="L32" s="45"/>
       <c r="M32" s="54"/>
       <c r="N32" s="30"/>
-      <c r="O32" s="201"/>
+      <c r="O32" s="171"/>
       <c r="P32" s="54"/>
       <c r="Q32" s="30"/>
       <c r="R32" s="45"/>
@@ -2407,10 +2406,10 @@
       <c r="V32" s="90"/>
     </row>
     <row r="33" spans="1:22" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="173" t="s">
+      <c r="A33" s="179" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="173" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -2437,8 +2436,8 @@
       <c r="V33" s="90"/>
     </row>
     <row r="34" spans="1:22" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="173"/>
-      <c r="B34" s="166"/>
+      <c r="A34" s="179"/>
+      <c r="B34" s="174"/>
       <c r="C34" s="19" t="s">
         <v>1</v>
       </c>
@@ -2452,8 +2451,8 @@
       <c r="T34" s="94"/>
     </row>
     <row r="35" spans="1:22" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="173"/>
-      <c r="B35" s="166" t="s">
+      <c r="A35" s="179"/>
+      <c r="B35" s="174" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -2469,8 +2468,8 @@
       <c r="T35" s="97"/>
     </row>
     <row r="36" spans="1:22" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="173"/>
-      <c r="B36" s="180"/>
+      <c r="A36" s="179"/>
+      <c r="B36" s="175"/>
       <c r="C36" s="134" t="s">
         <v>1</v>
       </c>
@@ -2493,10 +2492,10 @@
       <c r="T36" s="151"/>
     </row>
     <row r="37" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="186" t="s">
+      <c r="A37" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="183" t="s">
+      <c r="B37" s="188" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="21" t="s">
@@ -2523,34 +2522,34 @@
       <c r="V37" s="6"/>
     </row>
     <row r="38" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="187"/>
-      <c r="B38" s="184"/>
+      <c r="A38" s="182"/>
+      <c r="B38" s="189"/>
       <c r="C38" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="104"/>
-      <c r="F38" s="189"/>
-      <c r="G38" s="190"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="160"/>
       <c r="H38" s="104"/>
-      <c r="I38" s="189"/>
-      <c r="J38" s="190"/>
+      <c r="I38" s="159"/>
+      <c r="J38" s="160"/>
       <c r="K38" s="104"/>
       <c r="L38" s="43"/>
       <c r="M38" s="53"/>
       <c r="N38" s="8"/>
       <c r="O38" s="34"/>
-      <c r="P38" s="190"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="34"/>
+      <c r="P38" s="160"/>
+      <c r="Q38" s="104"/>
+      <c r="R38" s="159"/>
       <c r="S38" s="33"/>
       <c r="T38" s="34"/>
       <c r="U38" s="101"/>
       <c r="V38" s="6"/>
     </row>
     <row r="39" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="187"/>
-      <c r="B39" s="166" t="s">
+      <c r="A39" s="182"/>
+      <c r="B39" s="174" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -2577,23 +2576,23 @@
       <c r="V39" s="6"/>
     </row>
     <row r="40" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="187"/>
-      <c r="B40" s="166"/>
+      <c r="A40" s="182"/>
+      <c r="B40" s="174"/>
       <c r="C40" s="83" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="189"/>
+      <c r="F40" s="159"/>
       <c r="G40" s="53"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="189"/>
+      <c r="I40" s="159"/>
       <c r="J40" s="53"/>
       <c r="K40" s="8"/>
-      <c r="L40" s="189"/>
+      <c r="L40" s="159"/>
       <c r="M40" s="53"/>
       <c r="N40" s="8"/>
-      <c r="O40" s="189"/>
+      <c r="O40" s="159"/>
       <c r="P40" s="33"/>
       <c r="Q40" s="10"/>
       <c r="R40" s="34"/>
@@ -2603,8 +2602,8 @@
       <c r="V40" s="6"/>
     </row>
     <row r="41" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="187"/>
-      <c r="B41" s="166" t="s">
+      <c r="A41" s="182"/>
+      <c r="B41" s="174" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="18" t="s">
@@ -2631,8 +2630,8 @@
       <c r="V41" s="6"/>
     </row>
     <row r="42" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="188"/>
-      <c r="B42" s="181"/>
+      <c r="A42" s="183"/>
+      <c r="B42" s="177"/>
       <c r="C42" s="20" t="s">
         <v>1</v>
       </c>
@@ -2650,17 +2649,17 @@
       <c r="O42" s="76"/>
       <c r="P42" s="37"/>
       <c r="Q42" s="12"/>
-      <c r="R42" s="76"/>
+      <c r="R42" s="105"/>
       <c r="S42" s="37"/>
       <c r="T42" s="76"/>
       <c r="U42" s="101"/>
       <c r="V42" s="6"/>
     </row>
     <row r="43" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="173" t="s">
+      <c r="A43" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="170" t="s">
+      <c r="B43" s="176" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="18" t="s">
@@ -2687,8 +2686,8 @@
       <c r="V43" s="6"/>
     </row>
     <row r="44" spans="1:22" s="5" customFormat="1" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="162"/>
-      <c r="B44" s="181"/>
+      <c r="A44" s="180"/>
+      <c r="B44" s="177"/>
       <c r="C44" s="20" t="s">
         <v>1</v>
       </c>
@@ -2713,7 +2712,7 @@
       <c r="V44" s="6"/>
     </row>
     <row r="45" spans="1:22" s="5" customFormat="1" ht="68.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="176"/>
+      <c r="A45" s="172"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="3"/>
@@ -2736,12 +2735,12 @@
       <c r="U45" s="102"/>
     </row>
     <row r="46" spans="1:22" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="176"/>
+      <c r="A46" s="172"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:22" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="176"/>
+      <c r="A47" s="172"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="3"/>
@@ -2763,12 +2762,12 @@
       <c r="T47" s="3"/>
     </row>
     <row r="48" spans="1:22" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="176"/>
+      <c r="A48" s="172"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="176"/>
+      <c r="A49" s="172"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="3"/>
@@ -2790,12 +2789,12 @@
       <c r="T49" s="3"/>
     </row>
     <row r="50" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="176"/>
+      <c r="A50" s="172"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="176"/>
+      <c r="A51" s="172"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="3"/>
@@ -2817,12 +2816,12 @@
       <c r="T51" s="3"/>
     </row>
     <row r="52" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="176"/>
+      <c r="A52" s="172"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
     </row>
     <row r="53" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="176"/>
+      <c r="A53" s="172"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
@@ -2844,7 +2843,7 @@
       <c r="T53" s="3"/>
     </row>
     <row r="54" spans="1:20" s="5" customFormat="1" ht="68.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="176"/>
+      <c r="A54" s="172"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
     </row>
@@ -2869,6 +2868,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
@@ -2885,33 +2911,6 @@
     <mergeCell ref="A17:A28"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="19" orientation="portrait" r:id="rId1"/>
@@ -2928,6 +2927,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100545B467562A1CB4BAE1BBC04440EDC72" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="3d810219dc6ccac15e2c6825afbdd8b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8c96a1500b55a331f0d0926ba64a978c">
     <xsd:element name="properties">
@@ -3041,15 +3049,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8394405-7690-49B4-934B-E600857F4564}">
   <ds:schemaRefs>
@@ -3066,6 +3065,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6049531-61EF-4D8C-B24D-87FD4154C7C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A9A5433-7B0F-449A-9F76-1C68E6C13404}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3079,12 +3086,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6049531-61EF-4D8C-B24D-87FD4154C7C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>